<commit_message>
Minor fix for phone survey
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/Questionnaires/RF QRY [GLOBAL preprod].xlsx
+++ b/ADtests/Resources/Extra files/Questionnaires/RF QRY [GLOBAL preprod].xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="162">
   <si>
     <t>#</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>Question description Q1 (Qtype: Custom [DType: Check boxes] Review ID: $[203]$ )</t>
+  </si>
+  <si>
+    <t>YES+</t>
   </si>
 </sst>
 </file>
@@ -956,10 +959,10 @@
   <dimension ref="A1:BB112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="M21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3976,7 +3979,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="4"/>

</xml_diff>